<commit_message>
finished scripts and plots
</commit_message>
<xml_diff>
--- a/scbench_results.xlsx
+++ b/scbench_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_VN_Hausarbeit\DockerCEPH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE65CFA-4149-4614-89D8-465AF7F8057D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212B25F7-9F3B-4705-9E7B-2250ECC351CF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11715" yWindow="435" windowWidth="30510" windowHeight="19290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1650" yWindow="285" windowWidth="30510" windowHeight="19290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="4" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="108">
   <si>
     <t>hints</t>
   </si>
@@ -341,6 +341,24 @@
   <si>
     <t>Read Rand</t>
   </si>
+  <si>
+    <t>Values Calculated</t>
+  </si>
+  <si>
+    <t>Value Calculated</t>
+  </si>
+  <si>
+    <t>avg bandwidth</t>
+  </si>
+  <si>
+    <t>stddev bandwidth</t>
+  </si>
+  <si>
+    <t>max bandwidth</t>
+  </si>
+  <si>
+    <t>stddev latency</t>
+  </si>
 </sst>
 </file>
 
@@ -482,7 +500,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -668,6 +686,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -829,10 +853,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1188,10 +1213,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{530BADA9-B961-45DE-AC01-8A17953B5A8B}">
-  <dimension ref="H2:K46"/>
+  <dimension ref="H2:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U16" sqref="U16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="O39" sqref="O39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1619,7 +1644,7 @@
         <v>3.3467000000000002E-3</v>
       </c>
     </row>
-    <row r="34" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H34" s="2" t="s">
         <v>101</v>
       </c>
@@ -1633,7 +1658,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H35" t="s">
         <v>79</v>
       </c>
@@ -1647,7 +1672,7 @@
         <v>60.796900000000001</v>
       </c>
     </row>
-    <row r="36" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H36" t="s">
         <v>98</v>
       </c>
@@ -1661,7 +1686,7 @@
         <v>3702</v>
       </c>
     </row>
-    <row r="37" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H37" t="s">
         <v>99</v>
       </c>
@@ -1675,7 +1700,7 @@
         <v>4194304</v>
       </c>
     </row>
-    <row r="38" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H38" t="s">
         <v>80</v>
       </c>
@@ -1689,12 +1714,12 @@
         <v>4194304</v>
       </c>
     </row>
-    <row r="39" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H39" t="s">
         <v>81</v>
       </c>
       <c r="I39">
-        <v>1697.53</v>
+        <v>1702.3539999999998</v>
       </c>
       <c r="J39">
         <v>424.601</v>
@@ -1703,101 +1728,169 @@
         <v>243.565</v>
       </c>
     </row>
-    <row r="40" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H40" t="s">
+    <row r="40" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H40" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I40" s="3">
+        <v>10.385900249858</v>
+      </c>
+      <c r="J40" s="3">
+        <v>35.460804873622372</v>
+      </c>
+      <c r="K40" s="3">
+        <v>21.80546121993677</v>
+      </c>
+      <c r="L40" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="41" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H41" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="I41" s="3">
+        <v>1716</v>
+      </c>
+      <c r="J41" s="3">
+        <v>591.89800000000002</v>
+      </c>
+      <c r="K41" s="3">
+        <v>375.94299999999998</v>
+      </c>
+      <c r="L41" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="42" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H42" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="I42" s="3">
+        <v>0</v>
+      </c>
+      <c r="J42" s="3">
+        <v>0</v>
+      </c>
+      <c r="K42" s="3">
+        <v>0</v>
+      </c>
+      <c r="L42" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="43" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H43" t="s">
         <v>84</v>
       </c>
-      <c r="I40">
+      <c r="I43">
         <v>424</v>
       </c>
-      <c r="J40">
+      <c r="J43">
         <v>106</v>
       </c>
-      <c r="K40">
+      <c r="K43">
         <v>60</v>
       </c>
     </row>
-    <row r="41" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H41" t="s">
+    <row r="44" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H44" t="s">
         <v>85</v>
       </c>
-      <c r="I41">
+      <c r="I44">
         <v>9.6315500000000007</v>
       </c>
-      <c r="J41">
+      <c r="J44">
         <v>42.795499999999997</v>
       </c>
-      <c r="K41">
+      <c r="K44">
         <v>18.990100000000002</v>
       </c>
     </row>
-    <row r="42" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H42" t="s">
+    <row r="45" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H45" t="s">
         <v>86</v>
       </c>
-      <c r="I42">
+      <c r="I45">
         <v>432</v>
       </c>
-      <c r="J42">
+      <c r="J45">
         <v>180</v>
       </c>
-      <c r="K42">
+      <c r="K45">
         <v>113</v>
       </c>
     </row>
-    <row r="43" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H43" t="s">
+    <row r="46" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H46" t="s">
         <v>87</v>
       </c>
-      <c r="I43">
+      <c r="I46">
         <v>400</v>
       </c>
-      <c r="J43">
+      <c r="J46">
         <v>9</v>
       </c>
-      <c r="K43">
+      <c r="K46">
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H44" t="s">
+    <row r="47" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H47" t="s">
         <v>100</v>
       </c>
-      <c r="I44">
+      <c r="I47">
         <v>3.6549699999999997E-2</v>
       </c>
-      <c r="J44">
+      <c r="J47">
         <v>0.14726300000000001</v>
       </c>
-      <c r="K44">
+      <c r="K47">
         <v>0.26000099999999998</v>
       </c>
     </row>
-    <row r="45" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H45" t="s">
+    <row r="48" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H48" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I48" s="3">
+        <v>3.712216832298467E-4</v>
+      </c>
+      <c r="J48" s="3">
+        <v>1.762340435016066E-2</v>
+      </c>
+      <c r="K48" s="3">
+        <v>2.5047078326285055E-2</v>
+      </c>
+      <c r="L48" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="49" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H49" t="s">
         <v>89</v>
       </c>
-      <c r="I45">
+      <c r="I49">
         <v>0.20458699999999999</v>
       </c>
-      <c r="J45">
+      <c r="J49">
         <v>3.22601</v>
       </c>
-      <c r="K45">
+      <c r="K49">
         <v>3.94299</v>
       </c>
     </row>
-    <row r="46" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H46" t="s">
+    <row r="50" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H50" t="s">
         <v>90</v>
       </c>
-      <c r="I46">
+      <c r="I50">
         <v>3.2464899999999999E-3</v>
       </c>
-      <c r="J46">
+      <c r="J50">
         <v>2.6878900000000001E-3</v>
       </c>
-      <c r="K46">
+      <c r="K50">
         <v>2.6646600000000001E-3</v>
       </c>
     </row>
@@ -1809,10 +1902,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H523"/>
+  <dimension ref="A1:J523"/>
   <sheetViews>
     <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="I84" sqref="I84"/>
+      <selection activeCell="J85" sqref="J85:J89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3478,7 +3571,7 @@
         <v>244619</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>45</v>
       </c>
@@ -3492,7 +3585,7 @@
         <v>405276</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>47</v>
       </c>
@@ -3506,7 +3599,7 @@
         <v>115439</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>0</v>
       </c>
@@ -3515,7 +3608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>10</v>
       </c>
@@ -3540,8 +3633,15 @@
       <c r="H85" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I85">
+        <f>AVERAGE(E87:E96)</f>
+        <v>1702.3539999999998</v>
+      </c>
+      <c r="J85" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>0</v>
       </c>
@@ -3566,8 +3666,15 @@
       <c r="H86">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I86">
+        <f>_xlfn.STDEV.P(E87:E96)</f>
+        <v>10.385900249858</v>
+      </c>
+      <c r="J86" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>1</v>
       </c>
@@ -3592,8 +3699,15 @@
       <c r="H87">
         <v>3.5511399999999999E-2</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I87">
+        <f>MAX(E87:E96)</f>
+        <v>1716.4</v>
+      </c>
+      <c r="J87" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>2</v>
       </c>
@@ -3619,7 +3733,7 @@
         <v>3.5770099999999999E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>3</v>
       </c>
@@ -3644,8 +3758,15 @@
       <c r="H89">
         <v>3.60107E-2</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I89">
+        <f>_xlfn.STDEV.P(H87:H96)</f>
+        <v>3.712216832298467E-4</v>
+      </c>
+      <c r="J89" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>4</v>
       </c>
@@ -3671,7 +3792,7 @@
         <v>3.6014699999999997E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>5</v>
       </c>
@@ -3697,7 +3818,7 @@
         <v>3.6219500000000002E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>6</v>
       </c>
@@ -3723,7 +3844,7 @@
         <v>3.6512299999999998E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>7</v>
       </c>
@@ -3749,7 +3870,7 @@
         <v>3.6505299999999997E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>8</v>
       </c>
@@ -3775,7 +3896,7 @@
         <v>3.6657700000000001E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>9</v>
       </c>
@@ -3801,7 +3922,7 @@
         <v>3.6605400000000003E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>10</v>
       </c>
@@ -4052,10 +4173,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H406"/>
+  <dimension ref="A1:J406"/>
   <sheetViews>
     <sheetView topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="D92" sqref="D92:D107"/>
+      <selection activeCell="J129" sqref="J129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6687,7 +6808,7 @@
         <v>0.39032</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>19</v>
       </c>
@@ -6701,7 +6822,7 @@
         <v>1608</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>19</v>
       </c>
@@ -6712,7 +6833,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>50</v>
       </c>
@@ -6726,7 +6847,7 @@
         <v>94304</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>6</v>
       </c>
@@ -6740,7 +6861,7 @@
         <v>94304</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>25</v>
       </c>
@@ -6754,7 +6875,7 @@
         <v>0.96319999999999995</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>35</v>
       </c>
@@ -6765,7 +6886,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>28</v>
       </c>
@@ -6779,7 +6900,7 @@
         <v>0.67769999999999997</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>38</v>
       </c>
@@ -6790,7 +6911,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>40</v>
       </c>
@@ -6801,7 +6922,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>35</v>
       </c>
@@ -6815,7 +6936,7 @@
         <v>41836</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>45</v>
       </c>
@@ -6829,7 +6950,7 @@
         <v>90451</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>47</v>
       </c>
@@ -6843,7 +6964,7 @@
         <v>323903</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>0</v>
       </c>
@@ -6852,7 +6973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>10</v>
       </c>
@@ -6877,8 +6998,15 @@
       <c r="H127" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I127">
+        <f>AVERAGE(E129:E159)</f>
+        <v>446.27580645161288</v>
+      </c>
+      <c r="J127" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>0</v>
       </c>
@@ -6903,8 +7031,15 @@
       <c r="H128">
         <v>0</v>
       </c>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I128">
+        <f>_xlfn.STDEV.P(E129:E159)</f>
+        <v>35.460804873622372</v>
+      </c>
+      <c r="J128" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>1</v>
       </c>
@@ -6929,8 +7064,15 @@
       <c r="H129">
         <v>8.0787700000000004E-2</v>
       </c>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I129">
+        <f>MAX(E129:E159)</f>
+        <v>591.89800000000002</v>
+      </c>
+      <c r="J129" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>2</v>
       </c>
@@ -6956,7 +7098,7 @@
         <v>7.5735999999999998E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>3</v>
       </c>
@@ -6981,8 +7123,15 @@
       <c r="H131">
         <v>8.7403300000000003E-2</v>
       </c>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I131">
+        <f>_xlfn.STDEV.P(H129:H159)</f>
+        <v>1.762340435016066E-2</v>
+      </c>
+      <c r="J131" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>4</v>
       </c>
@@ -7008,7 +7157,7 @@
         <v>0.114263</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>5</v>
       </c>
@@ -7034,7 +7183,7 @@
         <v>0.12513299999999999</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>6</v>
       </c>
@@ -7060,7 +7209,7 @@
         <v>0.12939300000000001</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>7</v>
       </c>
@@ -7086,7 +7235,7 @@
         <v>0.12934399999999999</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>8</v>
       </c>
@@ -7112,7 +7261,7 @@
         <v>0.12712300000000001</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>9</v>
       </c>
@@ -7138,7 +7287,7 @@
         <v>0.13847999999999999</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>10</v>
       </c>
@@ -7164,7 +7313,7 @@
         <v>0.13030900000000001</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>11</v>
       </c>
@@ -7190,7 +7339,7 @@
         <v>0.12565999999999999</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>12</v>
       </c>
@@ -7216,7 +7365,7 @@
         <v>0.12709200000000001</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>13</v>
       </c>
@@ -7242,7 +7391,7 @@
         <v>0.13333300000000001</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>14</v>
       </c>
@@ -7268,7 +7417,7 @@
         <v>0.134352</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>15</v>
       </c>
@@ -7294,7 +7443,7 @@
         <v>0.133322</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>16</v>
       </c>
@@ -7917,10 +8066,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H236"/>
+  <dimension ref="A1:J236"/>
   <sheetViews>
-    <sheetView topLeftCell="A190" workbookViewId="0">
-      <selection activeCell="H128" sqref="H128"/>
+    <sheetView topLeftCell="A160" workbookViewId="0">
+      <selection activeCell="I165" sqref="I165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11601,7 +11750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>10</v>
       </c>
@@ -11626,8 +11775,15 @@
       <c r="H161" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I161">
+        <f>AVERAGE(E163:E222)</f>
+        <v>260.42055000000011</v>
+      </c>
+      <c r="J161" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>0</v>
       </c>
@@ -11652,8 +11808,15 @@
       <c r="H162">
         <v>0</v>
       </c>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I162">
+        <f>_xlfn.STDEV.P(E163:E222)</f>
+        <v>21.80546121993677</v>
+      </c>
+      <c r="J162" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>1</v>
       </c>
@@ -11678,8 +11841,15 @@
       <c r="H163">
         <v>0.11561200000000001</v>
       </c>
-    </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I163">
+        <f>MAX(E163:E222)</f>
+        <v>375.94299999999998</v>
+      </c>
+      <c r="J163" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>2</v>
       </c>
@@ -11705,7 +11875,7 @@
         <v>0.13209499999999999</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>3</v>
       </c>
@@ -11730,8 +11900,15 @@
       <c r="H165">
         <v>0.170935</v>
       </c>
-    </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I165">
+        <f>_xlfn.STDEV.P(H163:H222)</f>
+        <v>2.5047078326285055E-2</v>
+      </c>
+      <c r="J165" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>4</v>
       </c>
@@ -11757,7 +11934,7 @@
         <v>0.21812500000000001</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>5</v>
       </c>
@@ -11783,7 +11960,7 @@
         <v>0.21432399999999999</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>6</v>
       </c>
@@ -11809,7 +11986,7 @@
         <v>0.22276899999999999</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>7</v>
       </c>
@@ -11835,7 +12012,7 @@
         <v>0.23161499999999999</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>8</v>
       </c>
@@ -11861,7 +12038,7 @@
         <v>0.23139100000000001</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>9</v>
       </c>
@@ -11887,7 +12064,7 @@
         <v>0.216005</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>10</v>
       </c>
@@ -11913,7 +12090,7 @@
         <v>0.21909799999999999</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>11</v>
       </c>
@@ -11939,7 +12116,7 @@
         <v>0.22689500000000001</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>12</v>
       </c>
@@ -11965,7 +12142,7 @@
         <v>0.23066800000000001</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>13</v>
       </c>
@@ -11991,7 +12168,7 @@
         <v>0.242949</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
finished section about scbench
</commit_message>
<xml_diff>
--- a/scbench_results.xlsx
+++ b/scbench_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_VN_Hausarbeit\DockerCEPH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212B25F7-9F3B-4705-9E7B-2250ECC351CF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427BB977-A408-402D-B570-97BDA0C3963D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1650" yWindow="285" windowWidth="30510" windowHeight="19290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18705" yWindow="1290" windowWidth="30510" windowHeight="19290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="4" r:id="rId1"/>
@@ -1213,684 +1213,684 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{530BADA9-B961-45DE-AC01-8A17953B5A8B}">
-  <dimension ref="H2:L50"/>
+  <dimension ref="B2:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="O39" sqref="O39"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H2" s="2" t="s">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="I2" s="2">
+      <c r="C2" s="2">
         <v>10</v>
       </c>
-      <c r="J2" s="2">
+      <c r="D2" s="2">
         <v>30</v>
       </c>
-      <c r="K2" s="2">
+      <c r="E2" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H3" t="s">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>91</v>
       </c>
-      <c r="I3">
+      <c r="C3">
         <v>44.133099999999999</v>
       </c>
-      <c r="J3">
+      <c r="D3">
         <v>85.083200000000005</v>
       </c>
-      <c r="K3">
+      <c r="E3">
         <v>117.943</v>
       </c>
     </row>
-    <row r="4" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H4" t="s">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>92</v>
       </c>
-      <c r="I4">
+      <c r="C4">
         <v>19</v>
       </c>
-      <c r="J4">
+      <c r="D4">
         <v>54</v>
       </c>
-      <c r="K4">
+      <c r="E4">
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H5" t="s">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>93</v>
       </c>
-      <c r="I5">
+      <c r="C5">
         <v>4194304</v>
       </c>
-      <c r="J5">
+      <c r="D5">
         <v>4194304</v>
       </c>
-      <c r="K5">
+      <c r="E5">
         <v>4194304</v>
       </c>
     </row>
-    <row r="6" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H6" t="s">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>94</v>
       </c>
-      <c r="I6">
+      <c r="C6">
         <v>4194304</v>
       </c>
-      <c r="J6">
+      <c r="D6">
         <v>4194304</v>
       </c>
-      <c r="K6">
+      <c r="E6">
         <v>4194304</v>
       </c>
     </row>
-    <row r="7" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H7" t="s">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>81</v>
       </c>
-      <c r="I7">
+      <c r="C7">
         <v>1.7220599999999999</v>
       </c>
-      <c r="J7">
+      <c r="D7">
         <v>2.5386899999999999</v>
       </c>
-      <c r="K7">
+      <c r="E7">
         <v>2.3401000000000001</v>
       </c>
     </row>
-    <row r="8" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H8" t="s">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>95</v>
       </c>
-      <c r="I8">
+      <c r="C8">
         <v>0.91096299999999997</v>
       </c>
-      <c r="J8">
+      <c r="D8">
         <v>2.1305200000000002</v>
       </c>
-      <c r="K8">
+      <c r="E8">
         <v>1.0859700000000001</v>
       </c>
     </row>
-    <row r="9" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H9" t="s">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>82</v>
       </c>
-      <c r="I9">
+      <c r="C9">
         <v>4</v>
       </c>
-      <c r="J9">
+      <c r="D9">
         <v>14</v>
       </c>
-      <c r="K9">
+      <c r="E9">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H10" t="s">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>83</v>
       </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H11" t="s">
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>84</v>
       </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H12" t="s">
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>85</v>
       </c>
-      <c r="I12">
+      <c r="C12">
         <v>0.21070700000000001</v>
       </c>
-      <c r="J12">
+      <c r="D12">
         <v>0.473381</v>
       </c>
-      <c r="K12">
+      <c r="E12">
         <v>0.18490000000000001</v>
       </c>
     </row>
-    <row r="13" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H13" t="s">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>86</v>
       </c>
-      <c r="I13">
+      <c r="C13">
         <v>1</v>
       </c>
-      <c r="J13">
+      <c r="D13">
         <v>3</v>
       </c>
-      <c r="K13">
+      <c r="E13">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H14" t="s">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>87</v>
       </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H15" t="s">
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>88</v>
       </c>
-      <c r="I15">
+      <c r="C15">
         <v>28.848199999999999</v>
       </c>
-      <c r="J15">
+      <c r="D15">
         <v>31.3261</v>
       </c>
-      <c r="K15">
+      <c r="E15">
         <v>61.726999999999997</v>
       </c>
     </row>
-    <row r="16" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H16" t="s">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>96</v>
       </c>
-      <c r="I16">
+      <c r="C16">
         <v>16.270499999999998</v>
       </c>
-      <c r="J16">
+      <c r="D16">
         <v>16.053999999999998</v>
       </c>
-      <c r="K16">
+      <c r="E16">
         <v>11.387600000000001</v>
       </c>
     </row>
-    <row r="17" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H17" t="s">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>89</v>
       </c>
-      <c r="I17">
+      <c r="C17">
         <v>44.133000000000003</v>
       </c>
-      <c r="J17">
+      <c r="D17">
         <v>62.914400000000001</v>
       </c>
-      <c r="K17">
+      <c r="E17">
         <v>74.616799999999998</v>
       </c>
     </row>
-    <row r="18" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H18" t="s">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>90</v>
       </c>
-      <c r="I18">
+      <c r="C18">
         <v>1.64605</v>
       </c>
-      <c r="J18">
+      <c r="D18">
         <v>3.6095700000000002</v>
       </c>
-      <c r="K18">
+      <c r="E18">
         <v>36.218899999999998</v>
       </c>
     </row>
-    <row r="20" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H20" s="2" t="s">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="I20" s="2">
+      <c r="C20" s="2">
         <v>10</v>
       </c>
-      <c r="J20" s="2">
+      <c r="D20" s="2">
         <v>30</v>
       </c>
-      <c r="K20" s="2">
+      <c r="E20" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H21" t="s">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>79</v>
       </c>
-      <c r="I21">
+      <c r="C21">
         <v>4.2166000000000002E-2</v>
       </c>
-      <c r="J21">
+      <c r="D21">
         <v>2.1608000000000001</v>
       </c>
-      <c r="K21">
+      <c r="E21">
         <v>4.5196199999999997</v>
       </c>
     </row>
-    <row r="22" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H22" t="s">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>98</v>
       </c>
-      <c r="I22">
+      <c r="C22">
         <v>19</v>
       </c>
-      <c r="J22">
+      <c r="D22">
         <v>54</v>
       </c>
-      <c r="K22">
+      <c r="E22">
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H23" t="s">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>99</v>
       </c>
-      <c r="I23">
+      <c r="C23">
         <v>4194304</v>
       </c>
-      <c r="J23">
+      <c r="D23">
         <v>4194304</v>
       </c>
-      <c r="K23">
+      <c r="E23">
         <v>4194304</v>
       </c>
     </row>
-    <row r="24" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H24" t="s">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>80</v>
       </c>
-      <c r="I24">
+      <c r="C24">
         <v>4194304</v>
       </c>
-      <c r="J24">
+      <c r="D24">
         <v>4194304</v>
       </c>
-      <c r="K24">
+      <c r="E24">
         <v>4194304</v>
       </c>
     </row>
-    <row r="25" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H25" t="s">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
         <v>81</v>
       </c>
-      <c r="I25">
+      <c r="C25">
         <v>1802.4</v>
       </c>
-      <c r="J25">
+      <c r="D25">
         <v>99.963200000000001</v>
       </c>
-      <c r="K25">
+      <c r="E25">
         <v>64.067099999999996</v>
       </c>
     </row>
-    <row r="26" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H26" t="s">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
         <v>84</v>
       </c>
-      <c r="I26">
+      <c r="C26">
         <v>450</v>
       </c>
-      <c r="J26">
+      <c r="D26">
         <v>24</v>
       </c>
-      <c r="K26">
+      <c r="E26">
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H27" t="s">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
         <v>85</v>
       </c>
-      <c r="I27">
-        <v>0</v>
-      </c>
-      <c r="J27">
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
         <v>17.677700000000002</v>
       </c>
-      <c r="K27">
+      <c r="E27">
         <v>11.269399999999999</v>
       </c>
     </row>
-    <row r="28" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H28" t="s">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
         <v>86</v>
       </c>
-      <c r="I28">
-        <v>18</v>
-      </c>
-      <c r="J28">
+      <c r="C28">
+        <v>18</v>
+      </c>
+      <c r="D28">
         <v>39</v>
       </c>
-      <c r="K28">
+      <c r="E28">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H29" t="s">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
         <v>87</v>
       </c>
-      <c r="I29">
-        <v>18</v>
-      </c>
-      <c r="J29">
+      <c r="C29">
+        <v>18</v>
+      </c>
+      <c r="D29">
         <v>14</v>
       </c>
-      <c r="K29">
+      <c r="E29">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H30" t="s">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
         <v>100</v>
       </c>
-      <c r="I30">
+      <c r="C30">
         <v>2.4461900000000002E-2</v>
       </c>
-      <c r="J30">
+      <c r="D30">
         <v>0.41836000000000001</v>
       </c>
-      <c r="K30">
+      <c r="E30">
         <v>0.77932900000000005</v>
       </c>
     </row>
-    <row r="31" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H31" t="s">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>89</v>
       </c>
-      <c r="I31">
+      <c r="C31">
         <v>4.0527599999999997E-2</v>
       </c>
-      <c r="J31">
+      <c r="D31">
         <v>1.9045099999999999</v>
       </c>
-      <c r="K31">
+      <c r="E31">
         <v>4.0879700000000003</v>
       </c>
     </row>
-    <row r="32" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H32" t="s">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
         <v>90</v>
       </c>
-      <c r="I32">
+      <c r="C32">
         <v>0.115439</v>
       </c>
-      <c r="J32">
+      <c r="D32">
         <v>3.2390299999999999E-3</v>
       </c>
-      <c r="K32">
+      <c r="E32">
         <v>3.3467000000000002E-3</v>
       </c>
     </row>
-    <row r="34" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H34" s="2" t="s">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="I34" s="2">
+      <c r="C34" s="2">
         <v>10</v>
       </c>
-      <c r="J34" s="2">
+      <c r="D34" s="2">
         <v>30</v>
       </c>
-      <c r="K34" s="2">
+      <c r="E34" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H35" t="s">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
         <v>79</v>
       </c>
-      <c r="I35">
+      <c r="C35">
         <v>10.0381</v>
       </c>
-      <c r="J35">
+      <c r="D35">
         <v>31.172799999999999</v>
       </c>
-      <c r="K35">
+      <c r="E35">
         <v>60.796900000000001</v>
       </c>
     </row>
-    <row r="36" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H36" t="s">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
         <v>98</v>
       </c>
-      <c r="I36">
+      <c r="C36">
         <v>4260</v>
       </c>
-      <c r="J36">
+      <c r="D36">
         <v>3309</v>
       </c>
-      <c r="K36">
+      <c r="E36">
         <v>3702</v>
       </c>
     </row>
-    <row r="37" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H37" t="s">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
         <v>99</v>
       </c>
-      <c r="I37">
+      <c r="C37">
         <v>4194304</v>
       </c>
-      <c r="J37">
+      <c r="D37">
         <v>4194304</v>
       </c>
-      <c r="K37">
+      <c r="E37">
         <v>4194304</v>
       </c>
     </row>
-    <row r="38" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H38" t="s">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
         <v>80</v>
       </c>
-      <c r="I38">
+      <c r="C38">
         <v>4194304</v>
       </c>
-      <c r="J38">
+      <c r="D38">
         <v>4194304</v>
       </c>
-      <c r="K38">
+      <c r="E38">
         <v>4194304</v>
       </c>
     </row>
-    <row r="39" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H39" t="s">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
         <v>81</v>
       </c>
-      <c r="I39">
+      <c r="C39">
         <v>1702.3539999999998</v>
       </c>
-      <c r="J39">
+      <c r="D39">
         <v>424.601</v>
       </c>
-      <c r="K39">
+      <c r="E39">
         <v>243.565</v>
       </c>
     </row>
-    <row r="40" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H40" s="3" t="s">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="I40" s="3">
+      <c r="C40" s="3">
         <v>10.385900249858</v>
       </c>
-      <c r="J40" s="3">
+      <c r="D40" s="3">
         <v>35.460804873622372</v>
       </c>
-      <c r="K40" s="3">
+      <c r="E40" s="3">
         <v>21.80546121993677</v>
       </c>
-      <c r="L40" t="s">
+      <c r="F40" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="41" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H41" s="3" t="s">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="I41" s="3">
+      <c r="C41" s="3">
         <v>1716</v>
       </c>
-      <c r="J41" s="3">
+      <c r="D41" s="3">
         <v>591.89800000000002</v>
       </c>
-      <c r="K41" s="3">
+      <c r="E41" s="3">
         <v>375.94299999999998</v>
       </c>
-      <c r="L41" t="s">
+      <c r="F41" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="42" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H42" s="3" t="s">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="I42" s="3">
-        <v>0</v>
-      </c>
-      <c r="J42" s="3">
-        <v>0</v>
-      </c>
-      <c r="K42" s="3">
-        <v>0</v>
-      </c>
-      <c r="L42" t="s">
+      <c r="C42" s="3">
+        <v>0</v>
+      </c>
+      <c r="D42" s="3">
+        <v>0</v>
+      </c>
+      <c r="E42" s="3">
+        <v>0</v>
+      </c>
+      <c r="F42" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="43" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H43" t="s">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
         <v>84</v>
       </c>
-      <c r="I43">
+      <c r="C43">
         <v>424</v>
       </c>
-      <c r="J43">
+      <c r="D43">
         <v>106</v>
       </c>
-      <c r="K43">
+      <c r="E43">
         <v>60</v>
       </c>
     </row>
-    <row r="44" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H44" t="s">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
         <v>85</v>
       </c>
-      <c r="I44">
+      <c r="C44">
         <v>9.6315500000000007</v>
       </c>
-      <c r="J44">
+      <c r="D44">
         <v>42.795499999999997</v>
       </c>
-      <c r="K44">
+      <c r="E44">
         <v>18.990100000000002</v>
       </c>
     </row>
-    <row r="45" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H45" t="s">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
         <v>86</v>
       </c>
-      <c r="I45">
+      <c r="C45">
         <v>432</v>
       </c>
-      <c r="J45">
+      <c r="D45">
         <v>180</v>
       </c>
-      <c r="K45">
+      <c r="E45">
         <v>113</v>
       </c>
     </row>
-    <row r="46" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H46" t="s">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
         <v>87</v>
       </c>
-      <c r="I46">
+      <c r="C46">
         <v>400</v>
       </c>
-      <c r="J46">
+      <c r="D46">
         <v>9</v>
       </c>
-      <c r="K46">
+      <c r="E46">
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H47" t="s">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
         <v>100</v>
       </c>
-      <c r="I47">
+      <c r="C47">
         <v>3.6549699999999997E-2</v>
       </c>
-      <c r="J47">
+      <c r="D47">
         <v>0.14726300000000001</v>
       </c>
-      <c r="K47">
+      <c r="E47">
         <v>0.26000099999999998</v>
       </c>
     </row>
-    <row r="48" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H48" s="3" t="s">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B48" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="I48" s="3">
+      <c r="C48" s="3">
         <v>3.712216832298467E-4</v>
       </c>
-      <c r="J48" s="3">
+      <c r="D48" s="3">
         <v>1.762340435016066E-2</v>
       </c>
-      <c r="K48" s="3">
+      <c r="E48" s="3">
         <v>2.5047078326285055E-2</v>
       </c>
-      <c r="L48" t="s">
+      <c r="F48" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="49" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H49" t="s">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
         <v>89</v>
       </c>
-      <c r="I49">
+      <c r="C49">
         <v>0.20458699999999999</v>
       </c>
-      <c r="J49">
+      <c r="D49">
         <v>3.22601</v>
       </c>
-      <c r="K49">
+      <c r="E49">
         <v>3.94299</v>
       </c>
     </row>
-    <row r="50" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H50" t="s">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
         <v>90</v>
       </c>
-      <c r="I50">
+      <c r="C50">
         <v>3.2464899999999999E-3</v>
       </c>
-      <c r="J50">
+      <c r="D50">
         <v>2.6878900000000001E-3</v>
       </c>
-      <c r="K50">
+      <c r="E50">
         <v>2.6646600000000001E-3</v>
       </c>
     </row>
@@ -8069,7 +8069,7 @@
   <dimension ref="A1:J236"/>
   <sheetViews>
     <sheetView topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="I165" sqref="I165"/>
+      <selection activeCell="J196" sqref="J196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>